<commit_message>
added Excel data operation method
</commit_message>
<xml_diff>
--- a/kenon-user-interface/data/userlist.xlsx
+++ b/kenon-user-interface/data/userlist.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>社員番号</t>
   </si>
@@ -33,33 +33,6 @@
   </si>
   <si>
     <t>管理権限</t>
-  </si>
-  <si>
-    <t>u0001</t>
-  </si>
-  <si>
-    <t>モミン</t>
-  </si>
-  <si>
-    <t>ウェブ開発</t>
-  </si>
-  <si>
-    <t>momin.ice16@gmail.com</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>u0002</t>
-  </si>
-  <si>
-    <t>ロビ</t>
-  </si>
-  <si>
-    <t>ロビー</t>
-  </si>
-  <si>
-    <t>shekmomin07@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -133,52 +106,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>